<commit_message>
Update weekly data and enable dynamic week handling (Week 5 ready)
</commit_message>
<xml_diff>
--- a/data/master/sku_master.xlsx
+++ b/data/master/sku_master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop\D\Nitesh\Weekly Report - B2B + B2C\FastAPI\data\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC45139A-AAFB-4E47-95D1-75008D1C6752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A31D1E-2279-4C91-9CAD-88695B106FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{117C6BDF-C413-4A9B-8C98-0B7CEC880D6C}"/>
   </bookViews>
@@ -5604,7 +5604,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>